<commit_message>
refresh each data except red background. debugObj improve, still don't work
</commit_message>
<xml_diff>
--- a/Copy of GUI tasks 14.5.19.xlsx
+++ b/Copy of GUI tasks 14.5.19.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0994251-EE9F-473A-98D0-2E59EF4710BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A839C9-3B2B-4265-82C1-8DC3921CEF69}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t xml:space="preserve"> improve design</t>
   </si>
   <si>
-    <t>Import/Export parameters to file</t>
-  </si>
-  <si>
     <t>Import export QA</t>
   </si>
   <si>
@@ -191,6 +188,10 @@
   </si>
   <si>
     <t>power out put command 12[1] on/off int</t>
+  </si>
+  <si>
+    <t>Import/Export parameters to file
+review open files…path</t>
   </si>
 </sst>
 </file>
@@ -325,12 +326,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3A73EACE-E3FC-47D1-996E-6BD74AD6279D}" name="Table3" displayName="Table3" ref="A1:K28" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K28" xr:uid="{66409B4D-524D-496E-8DC9-D3517C7828E7}">
     <filterColumn colId="8">
-      <filters>
-        <filter val="7"/>
-        <filter val="8"/>
-        <filter val="8.5"/>
-        <filter val="9"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:K28">
@@ -618,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6DC6D2-EEA8-404D-A697-FFE68C9873A0}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:K14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="A2:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,13 +636,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -659,24 +657,24 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="3">
@@ -692,19 +690,19 @@
         <v>9</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -721,7 +719,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -740,12 +738,12 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
@@ -759,10 +757,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
@@ -778,10 +776,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5">
@@ -801,10 +799,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="5"/>
@@ -820,13 +818,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -841,13 +839,13 @@
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -862,10 +860,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7"/>
@@ -881,10 +879,10 @@
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="5"/>
@@ -900,13 +898,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -923,13 +921,13 @@
     </row>
     <row r="14" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -944,13 +942,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -965,10 +963,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
@@ -984,10 +982,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
@@ -1003,7 +1001,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>5</v>
@@ -1028,10 +1026,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
@@ -1047,7 +1045,7 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>10</v>
@@ -1068,7 +1066,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>4</v>
@@ -1089,15 +1087,15 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -1114,12 +1112,12 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="3"/>
@@ -1133,12 +1131,12 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="3"/>
@@ -1152,12 +1150,12 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="3"/>
@@ -1171,15 +1169,15 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1192,9 +1190,9 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>11</v>
@@ -1213,12 +1211,12 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="3"/>

</xml_diff>